<commit_message>
Add color, size, and morphology relational tables
Included all relational tables as .xlsx and .csv file formats
</commit_message>
<xml_diff>
--- a/data/Color.xlsx
+++ b/data/Color.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Desktop/Microplastic_Data_Portal-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948DE347-FF21-3F46-A464-4770770EE4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F1613C-827F-754D-91B8-BB9207E69566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19120" windowHeight="17440" xr2:uid="{F59E8F64-BA9A-6946-BBE2-F0BCEBC1228F}"/>
+    <workbookView xWindow="-19460" yWindow="500" windowWidth="19460" windowHeight="27240" xr2:uid="{F59E8F64-BA9A-6946-BBE2-F0BCEBC1228F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="34">
   <si>
     <t>SampleID</t>
   </si>
@@ -47,12 +47,105 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>C.10.18520/cs/v117/i11/1874-1879</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>B1.10.18520/cs/v117/i11/1874-1879</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>B2.10.18520/cs/v117/i11/1874-1879</t>
+  </si>
+  <si>
+    <t>B3.10.18520/cs/v117/i11/1874-1879</t>
+  </si>
+  <si>
+    <t>B4.10.18520/cs/v117/i11/1874-1879</t>
+  </si>
+  <si>
+    <t>B5.10.18520/cs/v117/i11/1874-1879</t>
+  </si>
+  <si>
+    <t>transparent</t>
+  </si>
+  <si>
+    <t>AverageAll_10.1016/j.envres.2022.112855</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>TCQS.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>SHN.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>CHQ.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>CHH.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>ZHB.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>DAS.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>XHS.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>HNZ.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>TCH.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>WHH.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>Spr.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>Sum.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>Aut.10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>Win.10.1016/j.scitotenv.2021.148001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -82,8 +175,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,14 +493,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE9FBD0-5ECD-C040-94F4-4EA3987834E8}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95:D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -423,6 +519,1392 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.86299999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D67" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>29</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>29</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>30</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>30</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>18</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>31</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>19</v>
+      </c>
+      <c r="D85" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>31</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>32</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>32</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>19</v>
+      </c>
+      <c r="D91" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>32</v>
+      </c>
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>32</v>
+      </c>
+      <c r="B93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>33</v>
+      </c>
+      <c r="B95" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" t="s">
+        <v>18</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0.48149999999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>33</v>
+      </c>
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>19</v>
+      </c>
+      <c r="D97" s="1">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>33</v>
+      </c>
+      <c r="B98" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0.13250000000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>33</v>
+      </c>
+      <c r="B99" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="1">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>33</v>
+      </c>
+      <c r="B100" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0.15279999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>